<commit_message>
Dokoncane vse naloge pod vaja 2
</commit_message>
<xml_diff>
--- a/Excel/Vaja2/rezultati.xlsx
+++ b/Excel/Vaja2/rezultati.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\RP\Excel\Vaja2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gits\RP\Excel\Vaja2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB9B8A2-35D0-4264-BEB3-723851504BDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rezultati" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -223,7 +233,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1096,7 +1106,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1122,7 +1131,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1290,7 +1299,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sl-SI"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1316,9 +1325,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1383,7 +1390,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -1409,7 +1415,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1439,7 +1445,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sl-SI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1495,7 +1501,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1521,7 +1526,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1692,7 +1697,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1718,7 +1722,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="sl-SI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1756,7 +1760,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="900104704"/>
@@ -1813,7 +1817,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1839,7 +1842,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="sl-SI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1871,7 +1874,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="900103392"/>
@@ -1888,7 +1891,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1914,7 +1916,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1944,7 +1946,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sl-SI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3061,20 +3063,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3092,19 +3100,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3198,6 +3212,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3233,6 +3264,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3408,11 +3456,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>